<commit_message>
Taking comments between workbook sheets
</commit_message>
<xml_diff>
--- a/src/main/resources/comentarios.xlsx
+++ b/src/main/resources/comentarios.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="395">
   <si>
     <t xml:space="preserve">Las alitas, hamburguesas y la cerveza están bastante ricas.</t>
   </si>
@@ -1107,6 +1107,105 @@
   </si>
   <si>
     <t>Excelente lugar no pierdan la oportunidad de ir, todo súper rico y la zona esta bonita, además hay promociones en días específicos</t>
+  </si>
+  <si>
+    <t>Limpio, excelente atención y buena comida</t>
+  </si>
+  <si>
+    <t>Riquísimo las costillas , el elote  y la cerveza buen lugar para comer lo recomiendo ampliamente</t>
+  </si>
+  <si>
+    <t>Muy buen ambiente para ver el fútbol y cualquier deporte... muy buenas promociones !!!</t>
+  </si>
+  <si>
+    <t>Increíbles margaritas  y la comida rica</t>
+  </si>
+  <si>
+    <t>Tienen muy buen servicio y es un buen lugar para venir y ver un partido con amigos y familiares</t>
+  </si>
+  <si>
+    <t>Buen lugar para botanear con los amigos.</t>
+  </si>
+  <si>
+    <t>Excelente todo, servicio, higiene, todo con calidad y calidez</t>
+  </si>
+  <si>
+    <t>Cómo en ningún otro lugar, atención, limpieza y una cocina que me ha llevado a volver varias veces.</t>
+  </si>
+  <si>
+    <t>Excelente lugar buena atención y la comida tiene buen sabor</t>
+  </si>
+  <si>
+    <t>De todos los Chili's a los que he ido este es donde mejor me atienden.</t>
+  </si>
+  <si>
+    <t>Está muy limpio y atienden bien. La comida muy buena.</t>
+  </si>
+  <si>
+    <t>Buen lugar para compartir con los amigos</t>
+  </si>
+  <si>
+    <t>Buen lugar para ver algún evento deportivo</t>
+  </si>
+  <si>
+    <t>Un restaurante de gran sabor y variedad en sus deliciosos platillos, hamburguesas, alias, costillas, dedos de queso, ensaladas, cervezas, refrescos de refil, postres, etc.</t>
+  </si>
+  <si>
+    <t>Muy buen servicio, excelente atención, y muy rica la comida</t>
+  </si>
+  <si>
+    <t>Excelente atención del personal, amabilidad, empaticoa. Comida muy rica y buena presentación. Altamente recomendable.</t>
+  </si>
+  <si>
+    <t>Excelente trato al cliente de parte de todos los empleados</t>
+  </si>
+  <si>
+    <t>Excelente lugar para unas cervezas con los amigos o una platica amena con una hermosa mujer!!!!</t>
+  </si>
+  <si>
+    <t>Me encanta el sabor de su comida, la atención y el servicio super eficiente.  Ubicación buena y sin mayores contratiempos.</t>
+  </si>
+  <si>
+    <t>Gran ambiente y gran sabor en los alimentos</t>
+  </si>
+  <si>
+    <t>Buen servicio, comida y ambiente</t>
+  </si>
+  <si>
+    <t>Las margaritas.....son muy buenas</t>
+  </si>
+  <si>
+    <t>Tiene mucha variedad y un gran también te, perfecto para ir en familia!</t>
+  </si>
+  <si>
+    <t>Buen servicio, buenos platos y es muy tranquilo el lugar</t>
+  </si>
+  <si>
+    <t>Excelente servicio y alimentos deliciosos!</t>
+  </si>
+  <si>
+    <t>Muy buena atención, excelente comida, buenisimos tragos</t>
+  </si>
+  <si>
+    <t>De las mejores sucursales a las que he ido, la atención del personal es increíble, siempre al pendiente de si necesitas algo. Los alimentos calientes y bien servidos. Muy recomendable</t>
+  </si>
+  <si>
+    <t>Muy buen servicio. Atención rápida.  Las hamburguesas son muy buenas y la cerveza de barril es deliciosa</t>
+  </si>
+  <si>
+    <t>Excelente atención y todo rico.</t>
+  </si>
+  <si>
+    <t>Muy buen lugar, te atienden rápido y todo el tiempo están al pendiente de ti sin abrumar. La comida es deliciosa y abundante.</t>
+  </si>
+  <si>
+    <t>Siempre regreso aqui... Me encanta tanto comida como servicio ... Recomiendo %100</t>
+  </si>
+  <si>
+    <t>un lugar muy recomendable además de que la comida es deliciosa y se ofrece una muy amplia barra de bebidas.</t>
+  </si>
+  <si>
+    <t>Muy buen lugar para pasar un excelente rato</t>
   </si>
 </sst>
 </file>
@@ -1207,7 +1306,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A305"/>
+  <dimension ref="A1:A270"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A309" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A311" activeCellId="0" sqref="A311"/>
@@ -2566,181 +2665,6 @@
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="1" t="s">
         <v>266</v>
-      </c>
-    </row>
-    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A294" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A295" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A296" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A297" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A298" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A300" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A301" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A302" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A303" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A305" s="1" t="s">
-        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -2759,7 +2683,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A55"/>
+  <dimension ref="A1:A90"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
@@ -2769,276 +2693,451 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>361</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>360</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>359</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>358</v>
+        <v>392</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
         <v>357</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>342</v>
+        <v>307</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>343</v>
+        <v>308</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>344</v>
+        <v>309</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>345</v>
+        <v>310</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>346</v>
+        <v>311</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>347</v>
+        <v>312</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>348</v>
+        <v>313</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>349</v>
+        <v>314</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>350</v>
+        <v>315</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>351</v>
+        <v>316</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>352</v>
+        <v>317</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>353</v>
+        <v>318</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>354</v>
+        <v>319</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>355</v>
+        <v>320</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
         <v>356</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixing gitignore file and don't shift rows when target sheet is empty
</commit_message>
<xml_diff>
--- a/src/main/resources/comentarios.xlsx
+++ b/src/main/resources/comentarios.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="445">
   <si>
     <t xml:space="preserve">Las alitas, hamburguesas y la cerveza están bastante ricas.</t>
   </si>
@@ -1206,6 +1206,156 @@
   </si>
   <si>
     <t>Muy buen lugar para pasar un excelente rato</t>
+  </si>
+  <si>
+    <t>La atención aquí es buenísima, además de que no hay que esperar tanto para ingresar al lugar.</t>
+  </si>
+  <si>
+    <t>Excelente!!!! Alimentos de primera y sobre todo un gran servicio</t>
+  </si>
+  <si>
+    <t>Completamente recomendable, la atención es rápida no te hacen esperar, las costillas, con una cerveza son una buena combinación</t>
+  </si>
+  <si>
+    <t>Los alimentos muy buenos y la atención de tofo el personal fue excelente; muy buena experiencia en esta sucursal.</t>
+  </si>
+  <si>
+    <t>muy buen lugar, la comida es muy rica, la atencion muy buena y los precios son adecuados</t>
+  </si>
+  <si>
+    <t>Todo muy rico vale la pena pagar sus precios</t>
+  </si>
+  <si>
+    <t>Súper rico, un lugar muy bonito y excelente servicio</t>
+  </si>
+  <si>
+    <t>Muy buen servicio los meseros atienden excelente y los alimentos perfectos</t>
+  </si>
+  <si>
+    <t>Es la primera vez que voy, la atencion y la comida buena. Los elotes deliciosos, la cerveza fría!!</t>
+  </si>
+  <si>
+    <t>Muy amables al atender y servicio súper rápido</t>
+  </si>
+  <si>
+    <t>Muy ricos alimentos y buen precio.</t>
+  </si>
+  <si>
+    <t>Lugar agradable, buen espacio, buena comida, atención rápida y amable</t>
+  </si>
+  <si>
+    <t>Una hamburguesa excepcional. A un precio razonable dada su calidad.</t>
+  </si>
+  <si>
+    <t>Deliciosas hamburguesas de las mejores de cdmx</t>
+  </si>
+  <si>
+    <t>Excelente servicio por parte del Staff !!</t>
+  </si>
+  <si>
+    <t>La comida es muy buena y el servicio es rápido y muy bueno</t>
+  </si>
+  <si>
+    <t>Un estándar de calidad y servicio los alimentos bien como siempre</t>
+  </si>
+  <si>
+    <t>Se come rico y servicio rapido</t>
+  </si>
+  <si>
+    <t>Buena atención y la calidad de los alimentos exquisita</t>
+  </si>
+  <si>
+    <t>Buen lugar, te atienden de maravilla</t>
+  </si>
+  <si>
+    <t>me encanta las ensaladas y las Margaritas</t>
+  </si>
+  <si>
+    <t>Excelente servicio cada vez que vamos</t>
+  </si>
+  <si>
+    <t>Los desayunos son deliciosos y los precios accesibles</t>
+  </si>
+  <si>
+    <t>Me encantan los alimentos y el ambiente relajado</t>
+  </si>
+  <si>
+    <t>Es uno de mis lugares favoritos</t>
+  </si>
+  <si>
+    <t>Esta tranquilo el lugar para cenar y platicar</t>
+  </si>
+  <si>
+    <t>El mejor Chilis de la zona!!! Obviamente por la atención brindada..</t>
+  </si>
+  <si>
+    <t>Me gustó mucho la hamburguesa con guacamole.</t>
+  </si>
+  <si>
+    <t>Sus papás y hamburguesas así como costillas son excelentes</t>
+  </si>
+  <si>
+    <t>Esta muy tranquilo, son rápidos y la comida esta muy buena.</t>
+  </si>
+  <si>
+    <t>Buena  comida, excelente ubicación, muy buen servicio, felicidades</t>
+  </si>
+  <si>
+    <t>Me encanta el salmón de Chili's, y el servicio como siempre: espectacular.</t>
+  </si>
+  <si>
+    <t>Sigue siendo un excelente servicio</t>
+  </si>
+  <si>
+    <t>Los alimentos bastante bien y la velocidad de atención mejoró muchísimo</t>
+  </si>
+  <si>
+    <t>Muy buena atención. Buen lugar para pasar un rato agradable</t>
+  </si>
+  <si>
+    <t>Excelente atención, los chicos súper serviciales y atentos.</t>
+  </si>
+  <si>
+    <t>La comida siempre de primera. Vale lo que cuesta.</t>
+  </si>
+  <si>
+    <t>Excelente atención rápida y eficiente comida muy rica.</t>
+  </si>
+  <si>
+    <t>Todo bien, buena comida y muchas pantallas para ver el fútbol</t>
+  </si>
+  <si>
+    <t>Costillitas deliciosas, bien servido, bebidas excelentes, muy recomendable</t>
+  </si>
+  <si>
+    <t>Me gustan sus costillaas bbq</t>
+  </si>
+  <si>
+    <t>Hoy estuvo muy bien el servicio y la comida deliciosa ,felicitaciones al Cheff!!!</t>
+  </si>
+  <si>
+    <t>La atención brindada es el plus del lugar.</t>
+  </si>
+  <si>
+    <t>Excelente siempre! Buen sabor, tamaño de las porciones y atención!</t>
+  </si>
+  <si>
+    <t>Muy amables y atentos, le ofrecieron alternativas vegetarianas a mis amigas</t>
+  </si>
+  <si>
+    <t>Excelente atención y ambiente 10 para los anfitriones</t>
+  </si>
+  <si>
+    <t>Todo muy limpio y atienden con prontitud y amabilidad</t>
+  </si>
+  <si>
+    <t>Muy buen lugar para salir con los amigos, la gerente del lugar estuvo al pendiente del servicio todo el tiempo</t>
+  </si>
+  <si>
+    <t>Un menú ideal, siempre teniendo excelente sabor y servicio</t>
+  </si>
+  <si>
+    <t>Excelente servicio, maravillosa calidez humana y deliciosos alimentos</t>
   </si>
 </sst>
 </file>
@@ -1306,7 +1456,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A270"/>
+  <dimension ref="A1:A360"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A309" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A311" activeCellId="0" sqref="A311"/>
@@ -1317,1353 +1467,1803 @@
     <col min="1" max="1" customWidth="true" hidden="false" style="1" width="8.45" collapsed="false" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
-        <v>88</v>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>90</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>91</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>92</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>93</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>94</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>95</v>
+        <v>6</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>96</v>
+        <v>7</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>100</v>
+        <v>11</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>104</v>
+        <v>15</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>105</v>
+        <v>17</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>106</v>
+        <v>18</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>107</v>
+        <v>19</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>108</v>
+        <v>20</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>109</v>
+        <v>21</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>111</v>
+        <v>23</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>112</v>
+        <v>24</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>114</v>
+        <v>26</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>115</v>
+        <v>27</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>116</v>
+        <v>28</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
-        <v>117</v>
+        <v>29</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>118</v>
+        <v>30</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>119</v>
+        <v>31</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>120</v>
+        <v>32</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>121</v>
+        <v>33</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>122</v>
+        <v>34</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
-        <v>123</v>
+        <v>35</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>124</v>
+        <v>36</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
-        <v>125</v>
+        <v>37</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>127</v>
+        <v>39</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
-        <v>129</v>
+        <v>41</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
-        <v>130</v>
+        <v>42</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>131</v>
+        <v>43</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>132</v>
+        <v>44</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>133</v>
+        <v>45</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>134</v>
+        <v>46</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>135</v>
+        <v>47</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
-        <v>136</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>137</v>
+        <v>48</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
-        <v>138</v>
+        <v>49</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>141</v>
+        <v>52</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>142</v>
+        <v>53</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>143</v>
+        <v>54</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>144</v>
+        <v>55</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
-        <v>145</v>
+        <v>56</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
-        <v>146</v>
+        <v>57</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
-        <v>149</v>
+        <v>60</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="s">
-        <v>150</v>
+        <v>61</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
-        <v>151</v>
+        <v>62</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
-        <v>152</v>
+        <v>63</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
-        <v>153</v>
+        <v>64</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="s">
-        <v>154</v>
+        <v>65</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="s">
-        <v>155</v>
+        <v>66</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
-        <v>156</v>
+        <v>67</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
-        <v>157</v>
+        <v>68</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
-        <v>158</v>
+        <v>69</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
-        <v>159</v>
+        <v>70</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="s">
-        <v>162</v>
+        <v>73</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="s">
-        <v>163</v>
+        <v>74</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
-        <v>164</v>
+        <v>75</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
-        <v>165</v>
+        <v>76</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
-        <v>166</v>
+        <v>77</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="s">
-        <v>167</v>
+        <v>78</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
-        <v>169</v>
+        <v>80</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="s">
-        <v>170</v>
+        <v>81</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="s">
-        <v>171</v>
+        <v>82</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="s">
-        <v>172</v>
+        <v>83</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="s">
-        <v>173</v>
+        <v>84</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="s">
-        <v>174</v>
+        <v>85</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="s">
-        <v>175</v>
+        <v>86</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="s">
-        <v>176</v>
+        <v>87</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="s">
-        <v>177</v>
+        <v>88</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
-        <v>178</v>
+        <v>89</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
-        <v>179</v>
+        <v>90</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
-        <v>180</v>
+        <v>91</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="s">
-        <v>181</v>
+        <v>92</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
-        <v>182</v>
+        <v>93</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
-        <v>183</v>
+        <v>94</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
-        <v>184</v>
+        <v>95</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="s">
-        <v>185</v>
+        <v>96</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="s">
-        <v>186</v>
+        <v>97</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="s">
-        <v>187</v>
+        <v>98</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="s">
-        <v>188</v>
+        <v>99</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="s">
-        <v>189</v>
+        <v>100</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="s">
-        <v>190</v>
+        <v>101</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="s">
-        <v>191</v>
+        <v>102</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="s">
-        <v>192</v>
+        <v>103</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="s">
-        <v>193</v>
+        <v>104</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
-        <v>194</v>
+        <v>69</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
-        <v>195</v>
+        <v>105</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="s">
-        <v>196</v>
+        <v>106</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="s">
-        <v>197</v>
+        <v>107</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="s">
-        <v>198</v>
+        <v>108</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="s">
-        <v>199</v>
+        <v>109</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="s">
-        <v>200</v>
+        <v>110</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="s">
-        <v>201</v>
+        <v>111</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
-        <v>202</v>
+        <v>112</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="s">
-        <v>203</v>
+        <v>113</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="s">
-        <v>204</v>
+        <v>114</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="s">
-        <v>205</v>
+        <v>115</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="s">
-        <v>206</v>
+        <v>116</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="s">
-        <v>207</v>
+        <v>117</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="s">
-        <v>208</v>
+        <v>118</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="s">
-        <v>209</v>
+        <v>119</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="s">
-        <v>210</v>
+        <v>120</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="s">
-        <v>210</v>
+        <v>121</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="s">
-        <v>211</v>
+        <v>122</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
-        <v>212</v>
+        <v>123</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="s">
-        <v>213</v>
+        <v>124</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="s">
-        <v>214</v>
+        <v>125</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="s">
-        <v>215</v>
+        <v>126</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="1" t="s">
-        <v>216</v>
+        <v>127</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="s">
-        <v>217</v>
+        <v>128</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="s">
-        <v>218</v>
+        <v>129</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="1" t="s">
-        <v>219</v>
+        <v>130</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="1" t="s">
-        <v>220</v>
+        <v>131</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="1" t="s">
-        <v>221</v>
+        <v>132</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="1" t="s">
-        <v>222</v>
+        <v>133</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="1" t="s">
-        <v>223</v>
+        <v>134</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="1" t="s">
-        <v>224</v>
+        <v>135</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="1" t="s">
-        <v>225</v>
+        <v>136</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="s">
-        <v>226</v>
+        <v>137</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="s">
-        <v>227</v>
+        <v>138</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="1" t="s">
-        <v>228</v>
+        <v>139</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="s">
-        <v>229</v>
+        <v>140</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="1" t="s">
-        <v>230</v>
+        <v>141</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="s">
-        <v>231</v>
+        <v>142</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="s">
-        <v>232</v>
+        <v>143</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="s">
-        <v>233</v>
+        <v>144</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="s">
-        <v>234</v>
+        <v>145</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="1" t="s">
-        <v>235</v>
+        <v>146</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="1" t="s">
-        <v>236</v>
+        <v>147</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="s">
-        <v>237</v>
+        <v>148</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="1" t="s">
-        <v>238</v>
+        <v>149</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="1" t="s">
-        <v>239</v>
+        <v>150</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="s">
-        <v>240</v>
+        <v>151</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="s">
-        <v>241</v>
+        <v>152</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="s">
-        <v>242</v>
+        <v>153</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="s">
-        <v>243</v>
+        <v>154</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="s">
-        <v>244</v>
+        <v>155</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="1" t="s">
-        <v>245</v>
+        <v>156</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="1" t="s">
-        <v>246</v>
+        <v>157</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="1" t="s">
-        <v>247</v>
+        <v>158</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="1" t="s">
-        <v>248</v>
+        <v>159</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="1" t="s">
-        <v>249</v>
+        <v>160</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="1" t="s">
-        <v>250</v>
+        <v>161</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="1" t="s">
-        <v>251</v>
+        <v>162</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="1" t="s">
-        <v>252</v>
+        <v>163</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="1" t="s">
-        <v>253</v>
+        <v>164</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="1" t="s">
-        <v>254</v>
+        <v>165</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="1" t="s">
-        <v>255</v>
+        <v>166</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="1" t="s">
-        <v>256</v>
+        <v>167</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="s">
-        <v>257</v>
+        <v>168</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="s">
-        <v>258</v>
+        <v>169</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="1" t="s">
-        <v>259</v>
+        <v>170</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="1" t="s">
-        <v>260</v>
+        <v>171</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="s">
-        <v>261</v>
+        <v>172</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="s">
-        <v>262</v>
+        <v>173</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="1" t="s">
-        <v>263</v>
+        <v>174</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="s">
-        <v>264</v>
+        <v>175</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="1" t="s">
-        <v>265</v>
+        <v>176</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A294" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A295" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A296" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A297" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A298" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A299" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A300" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A301" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A302" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A303" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A304" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A305" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A306" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A307" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A308" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A309" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A310" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A311" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A312" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A313" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A314" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A315" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A316" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A317" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A318" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A319" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A320" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A321" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A322" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A323" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A324" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A325" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A326" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A327" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A328" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A329" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A330" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A331" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A332" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A333" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A334" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A335" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A336" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A337" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A338" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A339" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A340" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A341" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A342" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A343" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A344" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A345" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A346" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A347" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A348" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A349" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A350" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A351" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A352" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A353" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A354" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A355" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A356" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A357" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A358" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A359" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A360" s="1" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2683,465 +3283,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A90"/>
+  <dimension ref="A1:A80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>